<commit_message>
Projeto finalizado com Flask
</commit_message>
<xml_diff>
--- a/produtos_ordenados.xlsx
+++ b/produtos_ordenados.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,1040 +465,1000 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mini Maquina De Lavar Roupa Portátil Dobrável Centrifuga 11l</t>
+          <t>Saco Para Até 10 Bolas / Porta Bolas Fio 4mm Branco</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>222.25</v>
+        <v>12.81</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_716948-MLB81818739364_012025-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_720045-MLU72700298625_112023-E.webp</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=X1ystcb41xamFz9w5ErWAmseIHY6WMpMjTwUXGHtZ2U0RXVJMzXjXtHCD%2BwuieYw9t%2FggdFhznauQ%2FfxhUkD9a84Z%2FtDvaQeZgWuOB27GpRZRsmcVYCyOtcvl%2B0orbqnUbWDB2hJmbg4vWRWftCz3fUQKEmXFe%2FH6BJEBn0EGSqYezPCZflODPHuUWQrJ0T0%2B%2FEjuWCkF81Q2F%2FsJd%2Fpb%2FlKrB024avIQ4Tv6NCbnNjNk8%2FHiFbE%2BzU32AghNDfWYNcs1JXY8iaAcKMSTkhi6zUlNwbAbyIKydCzJRL8%2BPVIEjDSKaGSoP3fr%2FfvoKlp4fltXHzHhyzj9ekaloOWVDT0QZPQwnMuZAj6rl2BCLtZnUoM3K%2B3zMYtiULydK2W25Oa3yVptgQHsAFlXCs4zZGyXYR1RzhLbI8NMU8q%2BHUtRxN7CUWx%2BfV5ERBm%2FPfCS%2BMCgxtdZSjR7kE9VGMEcOGQO4WNO6Tsya8iRcLsJDD%2B%2FhzcY7G8yQKxp5clI52VGdeOIYB1%2Behq%2BN9ve03%2Bz%2FGB7cvHPgqqbdg4R7RDRN5aaZpZO9XchxH1CHRlAFegV3uEcRrT8RfOLa005mdBtZl5iaR2u9ZtXXedX7SRCBeadpL7jrUM9MKKf06dw6muRJrycLUZm7tMPUz5W%2BNkBIiKAiXUCgpvr3rfCGXSsSE8lsm0a3VJMNfEcJPs02KuSlt0FXwB9vdYm8V18M1GQB61mq5LNDeL6deZWWEHq9MDPzXCQ6i%2FPIHiykt2C%2B06qN7usfD45k2Wk8zCCyWTTPBgCp4jzdUPzK5uIEgdhGEJzVfDfSgh1SKD0Az0rcRRObMC0GvP1dLtSeoL4YnlS29HFpug%2B5IKrDBee8uFYLG8nRaWEw%3D%3D&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22</t>
+          <t>https://www.mercadolivre.com.br/saco-para-ate-10-bolas-porta-bolas-fio-4mm-branco/p/MLB25996601#polycard_client=search-nordic&amp;searchVariation=MLB25996601&amp;wid=MLB4147585512&amp;position=5&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lavadora Semiautomática 110v 4kg Wanke Super Branca</t>
+          <t>Bola De Futebol Para Campo Tamanho 5 Petrin Presente Cor</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>418.9</v>
+        <v>18.37</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_649226-MLB82010457360_022025-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_859381-MLA81212900247_122024-E.webp</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=WYL6B8H8GdPuKyh8sEvikvMjegBvq7%2Bryw8Slc11M3KSJep9HVLDahVv6PmmZ2SRcTxkVOaJ2TJaIGNDkIyIW8sV5uqveDcZnbIAO0aIas1B24KJylQRuhKeP9%2FKY5%2BMqljfIQ8lyZ%2FRS%2F32PD%2B6FBjoe9xzW7op0gtmriceZlZGgN2eZcUlygLbmPMB1Abzj%2FZlrNJzYrCJGotBHGU6AylpuIr92ep9ytQhmyVcOdd5txt2Qfx1CsFJ4VswHpPMz609%2B5e5QQVMtsaLSTk43eqkG2Hi5dt1HsXU04tR43J2o0ksS%2Bqe2h%2BCGzDXS3rKbtnzXllr3jsUwSalFOrYWtyfe81GyrwJ%2BjnkptN0yJVuT61BeKXT3N0SQnfuDs%2FgUElp7N%2B0jcLsPyh%2BGqiGXxz4wYiUhWsHcSl5OBIajNJBC4snj8E1iH4p3m89c6DtCiDmfJVvbdY9QuRvO0s4eULy9lialCFtW%2F%2Fc48RXpa9Rh%2BeVmPBGTmi21xRduEh116OsZu%2BBv2blwUIj%2F1TJl6i61D2atroVPtC0uqpMnobgkkKKRmVrof5hRbbqgueEH%2FiMtD%2ByFzXuLsHcmS93yQg4CQzIWSoUWgCXEv5BMRmrY7iw7nopMLqxbPyFMMEKx4NRUFGcizPLb9Zy%2BL6wMFBsMr3NH7kcQIzDP4m24gRjtyV5nd2klKkt%2Fd7vwkEVyfo%2BDFApf0NBsgT0TYH7fXtNCWTQEAxHkv1YsFvtVKfTEjsCi%2BX7i1et5i3pG2nNqLskW8G%2F2quyMD1Aawl2F4ihF9ooAlPL4KeV5ofy0LQ%2Bj9zzWUruMrIED5cpUZaB4yAxId5IMBwoa5T3INsjY0vye3G6xX%2Faxtw%3D&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-para-campo-tamanho-5-petrin-presente-cor/p/MLB44556814#polycard_client=search-nordic&amp;searchVariation=MLB44556814&amp;wid=MLB4007228671&amp;position=39&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tanquinho Suggar Neo Turbilhão 8kg Le8002br 220v Cor Branco</t>
+          <t>Trave Futebol Gol Kit Mini Golzinho Infantil Brinquedo Bola</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>455.01</v>
+        <v>33.54</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_734374-MLU77348996425_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_764435-MLA79889067517_102024-E.webp</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/tanquinho-suggar-neo-turbilho-8kg-le8002br-220v-cor-branco/p/MLB36727621#polycard_client=search-nordic&amp;searchVariation=MLB36727621&amp;wid=MLB5057364952&amp;position=40&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/trave-futebol-gol-kit-mini-golzinho-infantil-brinquedo-bola/p/MLB41775954#polycard_client=search-nordic&amp;searchVariation=MLB41775954&amp;wid=MLB5118193404&amp;position=11&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Suggar Lavamax Eco LE8001BR tanquinho branco 110V</t>
+          <t>Tabela De Medição De Pressão, Medidor De Ponteiro De Futebol</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>477.63</v>
+        <v>38.31</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_903787-MLU77149873678_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_725638-CBT81594394892_012025-E.webp</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/suggar-lavamax-eco-le8001br-tanquinho-branco-110v/p/MLB35352522#polycard_client=search-nordic&amp;searchVariation=MLB35352522&amp;wid=MLB3864921779&amp;position=4&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/pressure-measurement-table-portable-football-pointer-gauge/p/MLB2009472856#polycard_client=search-nordic&amp;searchVariation=MLB2009472856&amp;wid=MLB4000139541&amp;position=9&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tanquinho Libell 20,5 Kg Com Lavagem Por Turbilhonamento Branca 110v</t>
+          <t>Bola Futebol Tamanho 5 Capotão + Bomba De Ar E Bico Cor Azul</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>529.9</v>
+        <v>39.99</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_829414-MLU78948300574_092024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_628564-MLU78026959026_082024-E.webp</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/tanquinho-libell-205-kg-com-lavagem-por-turbilhonamento-branca-110v/p/MLB38622511#polycard_client=search-nordic&amp;searchVariation=MLB38622511&amp;wid=MLB3792112525&amp;position=8&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-tamanho-5-capoto-bomba-de-ar-e-bico-cor-azul/p/MLB39157733#polycard_client=search-nordic&amp;searchVariation=MLB39157733&amp;wid=MLB3870171799&amp;position=30&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Libell 50020063 lavadora semiautomática prata 110V</t>
+          <t>Kit Bola De Vôlei + Bola De Futebol + Bomba Pró Sortidas</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>533.4</v>
+        <v>41.22</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_821628-MLU78253349546_082024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_702577-MLA82266657438_022025-E.webp</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/libell-50020063-lavadora-semiautomatica-prata-110v/p/MLB38501929#polycard_client=search-nordic&amp;searchVariation=MLB38501929&amp;wid=MLB4932140502&amp;position=3&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/kit-bola-de-vlei-bola-de-futebol-bomba-pro-sortidas/p/MLB46184165#polycard_client=search-nordic&amp;searchVariation=MLB46184165&amp;wid=MLB5292902016&amp;position=22&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lavadora Lavamax Eco 15kg Preta Suggar Cor Preto 220V</t>
+          <t>Bola De Vôlei 3.5 Texturizada Amarela Rainha Topper</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>547.48</v>
+        <v>44.99</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_890503-MLA80574682681_112024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_875461-MLU78119836106_082024-E.webp</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-lavamax-eco-15kg-preta-suggar-cor-preto-220v/p/MLB36969891#polycard_client=search-nordic&amp;searchVariation=MLB36969891&amp;wid=MLB4695470976&amp;position=44&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-vlei-35-texturizada-amarela-rainha-topper/p/MLB21012198#polycard_client=search-nordic&amp;searchVariation=MLB21012198&amp;wid=MLB3963193225&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tanquinho Colormaq 13kg Cor Branco 127V</t>
+          <t>Bola De Futebol Luke Sports Tamanho 5 Campo E Society Branca Cor Branco</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>579.99</v>
+        <v>48.29</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_847215-MLU72998814050_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_921199-MLA80927520322_122024-E.webp</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/tanquinho-colormaq-13kg-cor-branco-127v/p/MLB28654464#polycard_client=search-nordic&amp;searchVariation=MLB28654464&amp;wid=MLB4445963928&amp;position=29&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-luke-sports-tamanho-5-campo-e-society-branca-cor-branco/p/MLB44516604#polycard_client=search-nordic&amp;searchVariation=MLB44516604&amp;wid=MLB5214268684&amp;position=32&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Máquina de lavar semi-automática Tanquinho Colormaq 10kg 127V prata</t>
+          <t>10 Bolas De Vinil Futebol Dente De Leite C/ Cor Branco Com Preto</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>609.99</v>
+        <v>48.97</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_979428-MLU75194455651_032024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_785671-MLU77640619462_072024-E.webp</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-semi-automatica-tanquinho-colormaq-10kg-127v-prata/p/MLB14815389#polycard_client=search-nordic&amp;searchVariation=MLB14815389&amp;wid=MLB3985806643&amp;position=36&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/10-bolas-de-vinil-futebol-dente-de-leite-c-cor-branco-com-preto/p/MLB38350019#polycard_client=search-nordic&amp;searchVariation=MLB38350019&amp;wid=MLB3855446145&amp;position=24&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Máquina de lavar semi-automática Tanquinho Colormaq LCS 20kg 127V - prata</t>
+          <t>Bola De Futebol De Campo Slick 2020 Topper Cor Amarelo Neon/Preto</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>629.9</v>
+        <v>48.99</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_914751-MLA52222533871_102022-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_969183-MLU75988202853_042024-E.webp</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-semi-automatica-tanquinho-colormaq-lcs-20kg-127v-prata/p/MLB18925150#polycard_client=search-nordic&amp;searchVariation=MLB18925150&amp;wid=MLB5088434214&amp;position=5&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-slick-2020-topper-cor-amarelo-neonpreto/p/MLB19754376#polycard_client=search-nordic&amp;searchVariation=MLB19754376&amp;wid=MLB5277328830&amp;position=38&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lavadora de Roupas Semiautomática Tanquinho Colormaq Lcs 20kg Capacidade</t>
+          <t>Bola De Futebol Slick Campo Cor Azul/Branco/Preto Topper</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>629.9</v>
+        <v>50.72</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_776576-MLA79219948314_092024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_979047-MLU71168535619_082023-E.webp</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-de-roupas-semiautomatica-tanquinho-colormaq-lcs-20kg-capacidade/p/MLB18925149#polycard_client=search-nordic&amp;searchVariation=MLB18925149&amp;wid=MLB5088428664&amp;position=31&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-slick-campo-cor-azulbrancopreto-topper/p/MLB19765484#polycard_client=search-nordic&amp;searchVariation=MLB19765484&amp;wid=MLB5270990860&amp;position=35&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Máquina de lavar Roupas semi-automática Tanquinho Colormaq LCS 20kg 220V - prata</t>
+          <t>Bola Futebol Society Ótimo Custo Beneficio Peso Ideal Top Cor Azul</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>629.9</v>
+        <v>53.82</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_750158-MLA52231558421_112022-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_862896-MLU69453002841_052023-E.webp</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-roupas-semi-automatica-tanquinho-colormaq-lcs-20kg-220v-prata/p/MLB18925151#polycard_client=search-nordic&amp;searchVariation=MLB18925151&amp;wid=MLB5088434216&amp;position=35&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-society-otimo-custo-beneficio-peso-ideal-top-cor-azul/p/MLB23339357#polycard_client=search-nordic&amp;searchVariation=MLB23339357&amp;wid=MLB3923038695&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Electrolux 8,5kg Branca Turbo Economia com Jet&amp;Clean e Filtro Fiapos (LAC09) - 127V</t>
+          <t>Bola De Futebol de Campo Slick 24 Tecnofusion Multicor Topper</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>1489</v>
+        <v>53.99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_810765-MLU77347944455_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_722050-MLU76926100481_062024-E.webp</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-electrolux-85kg-branca-turbo-economia-com-jetclean-e-filtro-fiapos-lac09-127v/p/MLB8802700#polycard_client=search-nordic&amp;searchVariation=MLB8802700&amp;wid=MLB3608595237&amp;position=28&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-slick-24-tecnofusion-multicor-topper/p/MLB35378541#polycard_client=search-nordic&amp;searchVariation=MLB35378541&amp;wid=MLB3963108755&amp;position=40&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Electrolux 8,5kg Branca Turbo Economia com Jet&amp;Clean e Filtro Fiapos (LAC09) - 220V</t>
+          <t>Bola De Futebol De Campo Slick 2020 Topper</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>1489</v>
+        <v>54.99</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_684734-MLU77344393799_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_735756-MLB54078855256_022023-E.webp</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-electrolux-85kg-branca-turbo-economia-com-jetclean-e-filtro-fiapos-lac09-220v/p/MLB8802701#polycard_client=search-nordic&amp;searchVariation=MLB8802701&amp;wid=MLB2798035670&amp;position=49&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-slick-2020-topper/p/MLB22262774#polycard_client=search-nordic&amp;searchVariation=MLB22262774&amp;wid=MLB5270990842&amp;position=13&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Máquina de lavar Electrolux 10,5kg branca turbo 127V com Jet&amp;Clean e filtro fiapos LAC11</t>
+          <t>Bola De Futsal Slick 24 Câmara Airvility 6 Gomos Topper</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>1549</v>
+        <v>54.99</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_671377-MLU77136665638_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_790020-MLU75616505649_042024-E.webp</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-electrolux-105kg-branca-turbo-127v-com-jetclean-e-filtro-fiapos-lac11/p/MLB6352461#polycard_client=search-nordic&amp;searchVariation=MLB6352461&amp;wid=MLB2797980682&amp;position=33&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-24-cmara-airvility-6-gomos-topper/p/MLB35378564#polycard_client=search-nordic&amp;searchVariation=MLB35378564&amp;wid=MLB3963063089&amp;position=29&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Colormaq Máquina de lavar Roupas Automática LCA 12kg 127 V Cor Branco</t>
+          <t>Bola De Futebol Para Campo 22 I Topper Cor Branco/Verde Mar/Preto</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>1629</v>
+        <v>55.85</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_939876-MLU72826758422_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_967540-MLU69495823375_052023-E.webp</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/colormaq-maquina-de-lavar-roupas-automatica-lca-12kg-127-v-cor-branco/p/MLB15805357#polycard_client=search-nordic&amp;searchVariation=MLB15805357&amp;wid=MLB4334658152&amp;position=34&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-para-campo-22-i-topper-cor-brancoverde-marpreto/p/MLB22272252#polycard_client=search-nordic&amp;searchVariation=MLB22272252&amp;wid=MLB4198884500&amp;position=4&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Consul CWB09BB 9kg Branca com Dosagem Econômica e Ciclo Edredom 110V</t>
+          <t>Bola De Futebol Campo Slick Cup Topper</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>1679</v>
+        <v>59.15</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_998540-MLU72748459545_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_659913-MLA80298884457_102024-E.webp</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-consul-cwb09bb-9kg-branca-com-dosagem-econmica-e-ciclo-edredom-110v/p/MLB19690291#polycard_client=search-nordic&amp;searchVariation=MLB19690291&amp;wid=MLB5079884600&amp;position=42&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-campo-slick-cup-topper/p/MLB19698380#polycard_client=search-nordic&amp;searchVariation=MLB19698380&amp;wid=MLB5189140588&amp;position=8&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Midea MA512W130A 13kg Wave Agitator Branca 220v</t>
+          <t>Bola De Futsal Slick 22 Topper Cor Branco/Amarelo Neon/Azul</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>1699</v>
+        <v>59.2</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_755507-MLA79658397779_092024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_656329-MLB54078855245_022023-E.webp</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-midea-ma512w130a-13kgwaveagitatorbranca-220v/p/MLB38510489#polycard_client=search-nordic&amp;searchVariation=MLB38510489&amp;wid=MLB5084618562&amp;position=23&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-22-topper-cor-brancoamarelo-neonazul/p/MLB22262771#polycard_client=search-nordic&amp;searchVariation=MLB22262771&amp;wid=MLB3820042822&amp;position=12&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Máquina De Lavar 9kg Efficient Care Led09 Branco Electrolux 110V</t>
+          <t>Bola De Futsal Slick Cup Topper Cor Laranja/Azul Anodizado/Preto</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>1782</v>
+        <v>59.9</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_880633-MLU77190169068_072024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_882043-MLU75981819389_042024-E.webp</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-9kg-efficient-care-led09-branco-electrolux-110v/p/MLB37287174#polycard_client=search-nordic&amp;searchVariation=MLB37287174&amp;wid=MLB4918140572&amp;position=45&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-cup-topper-cor-laranjaazul-anodizadopreto/p/MLB19710248#polycard_client=search-nordic&amp;searchVariation=MLB19710248&amp;wid=MLB2889188605&amp;position=36&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Lavadora De Roupas Electrolux Essencial Care 11kg (les11) 220V</t>
+          <t>Topper Futsal Slick Bola Futebol Salão Branco Com Azul</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>1862</v>
+        <v>60.99</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_789965-MLU72646938325_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_880504-MLU71134471481_082023-E.webp</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-de-roupas-electrolux-essencial-care-11kg-les11-220v/p/MLB15950022#polycard_client=search-nordic&amp;searchVariation=MLB15950022&amp;wid=MLB2042425025&amp;position=32&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/topper-futsal-slick-bola-futebol-salo-branco-com-azul/p/MLB26148855#polycard_client=search-nordic&amp;searchVariation=MLB26148855&amp;wid=MLB3963093661&amp;position=17&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Cwn13ab 13kg Branca Consul Cor Branco 110v</t>
+          <t>Bola De Futebol Society Slick 2020 Cor Branco/Preto/Amarelo Tamanho Único Topper</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>1899</v>
+        <v>61.76</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_814381-MLU79216564271_092024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_869053-MLB51937100243_102022-E.webp</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-cwn13ab-13kg-branca-consul-cor-branco-110v/p/MLB38930889#polycard_client=search-nordic&amp;searchVariation=MLB38930889&amp;wid=MLB5120909810&amp;position=13&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-society-slick-2020-cor-brancopretoamarelo-tamanho-unico-topper/p/MLB19744266#polycard_client=search-nordic&amp;searchVariation=MLB19744266&amp;wid=MLB5222132312&amp;position=20&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Midea MA512W150A 15kg Wave Agitator Branca 127V</t>
+          <t>Bola De Futevolei Altinha N°5 Quadra Areia Pro Praia</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>1899</v>
+        <v>65.97</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_908960-MLA80879576175_112024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_645076-MLB82458925554_022025-E-bola-de-futevolei-altinha-n5-quadra-areia-pro-praia.webp</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-midea-ma512w150a-15kg-wave-agitator-branca-127v/p/MLB40383128#polycard_client=search-nordic&amp;searchVariation=MLB40383128&amp;wid=MLB5084646814&amp;position=9&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=mYpbkfZv%2BWrkHXFcJzH%2BLNwYdTR0CClKwqUNkB8gCyWC%2FkdDlw6z8okZwVrmsuyR2mvs0GYH0ptERW22b6tFsUz0f5KJyKt0nZlkml5NHIihom1Px0J1CrbZ6BSH%2FQTGQE6B9ax%2B8GkDXee%2B3gEdsQRcITpBPk4s%2Fw8gpWzkpb6nHYDnDCDl2xtI3hK1lB3Wd5%2F%2Fd%2F80G3ATney9LcSZw2H4xE2MA85NvXkt7eZqjfydIIsRHfEjNqfi%2FkCWbCW44xypAzY70XuE9F34Sb0BBB5IrTcC1McHT%2FQt4QIlLn5MravpRWVd4SjFa6QU9%2FCOQJCek3J%2BfhFmi6pNVPwdjvRnCYAj5w617jbLWvuC9BJT0I8D7bMaV8QDGZALYfTZOfGT97MfuUXaR8ghh0ObguNGxU55WI2FSBFhZdflUaZsCNlQoxpEcAePwzEG3z85QfUHPHfZqR5w0na0JYqMbdr4SD8yNvtmACVwSDGRi44oCy3mDQxN6SD%2B0ksm4DoC%2BV3xPf2OEQcAkZByaZrXT4%2B3gafEjiieOk%2FK3hq79iySWUkvbfQ9s%2FKjQRQuB2SFp7BdKa3JXs9ckJwlOhqDwF9W6qK6NtExi5tDMVlig4EIBE85sqQAg46ddNkNlAHoWDGbafgKjwSTAxNppif8QmfMEE%2B26ocAjnPEHS8rDpgCfzEUyAQrou8F0S38ZvEluacn6hROTtflt0mPDQE7axmgsZnO2W9VsgeQreDZnbUF1SNZwEQeM11LfwQqyyGH%2Bme8eNvc8LGIA8UlFpcKtslbO%2FoJPAGu4A%2B0tShxXMRtpBbPDC9usKwaFGuPT7W5MhE6hmd3jfwtV84NEsMGcnY5tzYenexutjdg&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Máquina De Lavar 15kg Electrolux Essential Care Com Cesto In Cor Branco 110V</t>
+          <t>Bola De Futevolei Altinha N°5 Quadra Areia Pro Praia</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>1899</v>
+        <v>65.97</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_933655-MLU77338245029_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_645076-MLB82458925554_022025-E-bola-de-futevolei-altinha-n5-quadra-areia-pro-praia.webp</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-15kg-electrolux-essential-care-com-cesto-in-cor-branco-110v/p/MLB19037310#polycard_client=search-nordic&amp;searchVariation=MLB19037310&amp;wid=MLB2820206240&amp;position=27&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4006687617-bola-de-futevolei-altinha-n5-quadra-areia-pro-praia-_JM?searchVariation=183156389516#polycard_client=search-nordic&amp;searchVariation=183156389516&amp;position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Cwn13ab 13kg Branca Consul Cor Branco 220v</t>
+          <t>Bola De Futevôlei Diadora Elite-r</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>1899</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_814381-MLU79216564271_092024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_777673-MLB74305800482_022024-E-bola-de-futevlei-diadora-elite-r.webp</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-cwn13ab-13kg-branca-consul-cor-branco-220v/p/MLB38473748#polycard_client=search-nordic&amp;searchVariation=MLB38473748&amp;wid=MLB5120871416&amp;position=18&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=FA2v80kO0Q62jIC3APOe8OLdHZosDSTo1hLLRyRzr90a4JOmG9fNJuYmnoO8wg22iqTmr27d%2BrK3sZOAMDcUxTXULya%2FuqG3Uce7FwirY265ddOp%2FaRo0%2FUfe1%2Fe8RReqaCkhX4gJYzGKk62Jq9YuTkU%2FZbzoSwUeYEBMevSBPog0Bu0gIxXMJ93cIk4gUOvWjnzprMXLSMEiSakhNXOETkZc5KUFk1bQXqKVFLpHWMuz2XLh68FPbRohnW7tl%2BCcmfgQvwQKhoklCxqKO8wcN%2B12x61YphpgBIMTsCsHnlUsyjm18ZhifBDehyGu9uKFLf5gpt612eYaSwpb3psZ42tp7JY20HPiQBPpcWki4%2FqHPJIE8iZwN9PD8PRPxmFi%2B%2F9jhfUYSfXKW7I6emq3gWPDPAro%2BtAPq1Mlbu1WvjcEOFDOeYK%2F4o56stlpSmFH4zTluHTF8HsKZqH49c8i6VjRDwLf4JiWGWPeyy5JuASJg7cJfmPAASSftaG%2B5b%2BFAQx5qMBbAgkFrIVkMakbpJyEXx8LKisH3WrSN3mVVhT%2Bal25Bev9FVuqCIkH5rpVvnIOIthHtGurHdG5%2FUMhpGuYitAJxoXDha%2FceYFueTm8Ya0XdxcZd4LtZXVUsnvCxj%2FjN%2B5R%2BqrYb4uyMOPasbyNJqMjg4nxO6hb6fRGkW5imtNH17dsnmSd22hBtwdRfUtVo6b7VeYEEiD72oR%2Bf2sqpC8IVbMa%2B5uV03kiM3O7Atg3Dc6%2FLHKx%2Blem1khGGw4rvQ51VV%2FLhtFT0uDGeA367TVDZlCRBGdGq%2F8EF4H0r0oG9GbdOGxqt7Ld0bygm%2FBhLfnOQ%3D%3D&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Electrolux 15kg Branca Essential Care com Cesto Inox e Jet&amp;Clean LED15 220v</t>
+          <t>Bola De Futevôlei Diadora Elite-r</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>1899</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_956915-MLU77118725640_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_777673-MLB74305800482_022024-E-bola-de-futevlei-diadora-elite-r.webp</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-electrolux-15kg-branca-essential-care-com-cesto-inox-e-jetclean-led15-220v/p/MLB19037311#polycard_client=search-nordic&amp;searchVariation=MLB19037311&amp;wid=MLB2820216493&amp;position=48&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-3705513048-bola-de-futevlei-diadora-elite-r-_JM?searchVariation=177953619994#polycard_client=search-nordic&amp;searchVariation=177953619994&amp;position=50&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lavadora De Roupas Philco 14kg Plr14a 127v</t>
+          <t>Bola De Futevôlei Diadora Elite-r Cor Amarelo</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>1906</v>
+        <v>74.92</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_935142-MLA80891116954_122024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_699842-MLU70081962810_062023-E.webp</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-de-roupas-philco-14kg-plr14a-127v/p/MLB44409031#polycard_client=search-nordic&amp;searchVariation=MLB44409031&amp;wid=MLB3934734385&amp;position=43&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevlei-diadora-elite-r-cor-amarelo/p/MLB21096382#polycard_client=search-nordic&amp;searchVariation=MLB21096382&amp;wid=MLB3383487155&amp;position=19&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Panasonic 12kg Titânio Na-f120b1t Cor Cinza 220V</t>
+          <t>Bola De Campo Topper Slick Gold Dourada Oficial Bomba De Ar</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>1939</v>
+        <v>74.95</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_670021-MLU77169983306_072024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_869593-MLB82719894389_022025-E-bola-de-campo-topper-slick-gold-dourada-oficial-bomba-de-ar.webp</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-panasonic-12kg-titnio-na-f120b1t-cor-cinza-220v/p/MLB18019527#polycard_client=search-nordic&amp;searchVariation=MLB18019527&amp;wid=MLB2025672291&amp;position=37&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-3987100373-bola-de-campo-topper-slick-gold-dourada-oficial-bomba-de-ar-_JM?searchVariation=183000579442#polycard_client=search-nordic&amp;searchVariation=183000579442&amp;position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lavadora Electrolux 12kg Com Dispenser Autolimpante Lac12 220V</t>
+          <t>Bola Para Futebol De Campo Bravo Xxiv Branco e Azul Penalty</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>1940</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_938210-MLA43368841128_092020-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_698520-MLU75981724023_042024-E.webp</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-electrolux-12kg-com-dispenser-autolimpante-lac12-220v/p/MLB8045008#polycard_client=search-nordic&amp;searchVariation=MLB8045008&amp;wid=MLB2042392929&amp;position=7&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-para-futebol-de-campo-bravo-xxiv-branco-e-azul-penalty/p/MLB27895686#polycard_client=search-nordic&amp;searchVariation=MLB27895686&amp;wid=MLB3951567371&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Lavadora Electrolux 12kg Com Dispenser Autolimpante Lac12 127V</t>
+          <t>Bola Futsal Penalty Rx 500 Xxiii Cor Azul</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>1942</v>
+        <v>78.90000000000001</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_635073-MLU72747733932_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_722195-MLU77108763060_062024-E.webp</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-electrolux-12kg-com-dispenser-autolimpante-lac12-127v/p/MLB8045007#polycard_client=search-nordic&amp;searchVariation=MLB8045007&amp;wid=MLB2042392928&amp;position=16&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futsal-penalty-rx-500-xxiii-cor-azul/p/MLB25820360#polycard_client=search-nordic&amp;searchVariation=MLB25820360&amp;wid=MLB3996965885&amp;position=16&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Consul Cwh12bb Branca 12kg com Dosagem Econômica e Ciclo Edredom 110V</t>
+          <t>Bola De Futebol Branco E Laranja De Campo Bravo Xxiv Penalty</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>1955</v>
+        <v>78.98999999999999</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_868571-MLU72748300995_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_764251-MLU75813169222_042024-E.webp</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-consul-cwh12bb-branca-12kg-com-dosagem-econmica-e-ciclo-edredom-110v/p/MLB19954281#polycard_client=search-nordic&amp;searchVariation=MLB19954281&amp;wid=MLB3270039764&amp;position=39&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-branco-e-laranja-de-campo-bravo-xxiv-penalty/p/MLB27893082#polycard_client=search-nordic&amp;searchVariation=MLB27893082&amp;wid=MLB5056295770&amp;position=23&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Lavadora De Roupas Electrolux Essencial Care 11kg (les11) 127V</t>
+          <t>Bola Para Futebol De Campo Líder Xxiv Cor Branco/Azul/Verde Penalty</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>1974</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_798413-MLA43117842453_082020-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_895518-MLU74287171999_012024-E.webp</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-de-roupas-electrolux-essencial-care-11kg-les11-127v/p/MLB15950021#polycard_client=search-nordic&amp;searchVariation=MLB15950021&amp;wid=MLB2042380330&amp;position=17&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-para-futebol-de-campo-lider-xxiv-cor-brancoazulverde-penalty/p/MLB30924589#polycard_client=search-nordic&amp;searchVariation=MLB30924589&amp;wid=MLB3937962097&amp;position=10&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Cwn15ab 15kg Branca Consul Cor Branco 110v</t>
+          <t>Bola Allpha Futsal Pró+ Madri Pu Maciez Treino Original</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>1999</v>
+        <v>106.69</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_835643-MLU78412371310_082024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_965545-MLB82741758954_032025-E-bola-allpha-futsal-pro-madri-pu-maciez-treino-original.webp</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-cwn15ab-15kg-branca-consul-cor-branco-110v/p/MLB39455938#polycard_client=search-nordic&amp;searchVariation=MLB39455938&amp;wid=MLB3834214575&amp;position=11&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4000309717-bola-allpha-futsal-pro-madri-pu-maciez-treino-original-_JM?searchVariation=183112590022#polycard_client=search-nordic&amp;searchVariation=183112590022&amp;position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Cwn15ab 15kg Branca Consul Cor Branco 220v</t>
+          <t>Bola de Futebol Penalty Society Lider XXIV Branco Laranja Azul 5</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>1999</v>
+        <v>111.71</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_764211-MLU78408768259_082024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_903645-MLU74833063908_032024-E.webp</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-cwn15ab-15kg-branca-consul-cor-branco-220v/p/MLB39328201#polycard_client=search-nordic&amp;searchVariation=MLB39328201&amp;wid=MLB3825557205&amp;position=19&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-penalty-society-lider-xxiv-branco-laranja-azul-5/p/MLB27892495#polycard_client=search-nordic&amp;searchVariation=MLB27892495&amp;wid=MLB3951591553&amp;position=18&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Electrolux 14kg Branca Essential Care com Cesto Inox e Jet&amp;Clean LED14 110V</t>
+          <t>Bola Society Líder Xxiv Pu Laminado 6 Gomos Penalty</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>2048</v>
+        <v>114.99</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_927128-MLU78108592086_082024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_609551-MLU78177695411_082024-E.webp</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-electrolux-14kg-branca-essential-care-com-cesto-inox-e-jetclean-led14-110v/p/MLB17920363#polycard_client=search-nordic&amp;searchVariation=MLB17920363&amp;wid=MLB2042425192&amp;position=21&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-society-lider-xxiv-pu-laminado-6-gomos-penalty/p/MLB27924191#polycard_client=search-nordic&amp;searchVariation=MLB27924191&amp;wid=MLB3938335813&amp;position=7&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Bwk13ab 13kg Branca Brastemp Cor Branco 110V</t>
+          <t>Bola De Futebol Corinthians Time Oficial Licenciada Timão</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>2093</v>
+        <v>119</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_713249-MLA72428771637_102023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_707361-MLB82839791767_032025-E-bola-de-futebol-corinthians-time-oficial-licenciada-timo.webp</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-bwk13ab-13kg-branca-brastemp-cor-branco-110v/p/MLB27592682#polycard_client=search-nordic&amp;searchVariation=MLB27592682&amp;wid=MLB4148593028&amp;position=20&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-3992563623-bola-de-futebol-corinthians-time-oficial-licenciada-timo-_JM?searchVariation=187103662249#polycard_client=search-nordic&amp;searchVariation=187103662249&amp;position=49&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Máquina De Lavar 14kg Essential Care LED14 Com Cesto Inox E Jet&amp;Clean Electrolux 220V</t>
+          <t>Bola Futevolei Altinha Ftv Ft5 Penta Futemesa Rio Cor Preto</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>2162</v>
+        <v>126.85</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_927128-MLU78108592086_082024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_764380-MLU73463308040_122023-E.webp</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-14kg-essential-care-led14-com-cesto-inox-e-jetclean-electrolux-220v/p/MLB17920364#polycard_client=search-nordic&amp;searchVariation=MLB17920364&amp;wid=MLB2042367533&amp;position=41&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futevolei-altinha-ftv-ft5-penta-futemesa-rio-cor-preto/p/MLB29123039#polycard_client=search-nordic&amp;searchVariation=MLB29123039&amp;wid=MLB4321183772&amp;position=28&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Máquina de Lavar NA-F170B7W Com Sistema Ciclone e Função Smartsense 17kg Cor Branca 127V</t>
+          <t>Bola 81 Dalponte Star Campo Costurada A Mão Original</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>2199</v>
+        <v>131</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_885462-MLU72748594615_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_947113-MLB45202965881_032021-E.webp</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-na-f170b7w-com-sistema-ciclone-e-funco-smartsense-17kg-cor-branca-127v/p/MLB23462525#polycard_client=search-nordic&amp;searchVariation=MLB23462525&amp;wid=MLB3351549387&amp;position=25&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-81-dalponte-star-campo-costurada-a-mo-original/p/MLB20563342#polycard_client=search-nordic&amp;searchVariation=MLB20563342&amp;wid=MLB4006264629&amp;position=26&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Na-f170b7wb 17kg Branca Panasonic 220v Cor Branco</t>
+          <t>Bola de futevolei Poker Rio Poker nº 5 Unidade x 1 unidades cor rosa e preto</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>2199</v>
+        <v>135</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_897025-MLU72748623701_112023-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_904045-MLU79036618824_092024-E.webp</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-na-f170b7wb-17kg-branca-panasonic-220v-cor-branco/p/MLB23458910#polycard_client=search-nordic&amp;searchVariation=MLB23458910&amp;wid=MLB3332415215&amp;position=46&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-unidade-x-1-unidades-cor-rosa-e-preto/p/MLB19698706#polycard_client=search-nordic&amp;searchVariation=MLB19698706&amp;wid=MLB5051108460&amp;position=34&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Bwk13a9 13kg Cinza Platinum Brastemp Cor Cinza-escuro 110V</t>
+          <t>Bola de Futevolei Poker Rio Poker nº 5 cor amarelo e preto</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>2202</v>
+        <v>139.29</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_630024-MLU74978359017_032024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_753390-MLU74696438844_022024-E.webp</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-bwk13a9-13kg-cinza-platinum-brastemp-cor-cinza-escuro-110v/p/MLB27950738#polycard_client=search-nordic&amp;searchVariation=MLB27950738&amp;wid=MLB4169866822&amp;position=22&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-cor-amarelo-e-preto/p/MLB19698709#polycard_client=search-nordic&amp;searchVariation=MLB19698709&amp;wid=MLB3889075523&amp;position=31&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Bwk13a9 13kg Cinza Platinum Brastemp Cor Cinza-escuro 220V</t>
+          <t>Bola de futevolei Poker Rio Poker nº 5 Unidade x 1 unidades cor branco e preto</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>2202</v>
+        <v>140.11</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_723323-MLU74842936884_032024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_773647-MLA79588973813_092024-E.webp</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-bwk13a9-13kg-cinza-platinum-brastemp-cor-cinza-escuro-220v/p/MLB27950739#polycard_client=search-nordic&amp;searchVariation=MLB27950739&amp;wid=MLB4169909966&amp;position=30&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-unidade-x-1-unidades-cor-branco-e-preto/p/MLB19698708#polycard_client=search-nordic&amp;searchVariation=MLB19698708&amp;wid=MLB3889079001&amp;position=33&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Bwf15ab 15kg Tira Manchas Branca Brastemp Cor Branco 110V</t>
+          <t>Bola Futevôlei Vulcanizada Pu Poker Original Branca/azul</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>2211</v>
+        <v>149.9</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_663713-MLU74979993323_032024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_601980-MLB83086122841_032025-E-bola-futevlei-vulcanizada-pu-poker-original-brancaazul.webp</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-bwf15ab-15kg-tira-manchas-branca-brastemp-cor-branco-110v/p/MLB26876403#polycard_client=search-nordic&amp;searchVariation=MLB26876403&amp;wid=MLB4106662150&amp;position=10&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-5318075606-bola-futevlei-vulcanizada-pu-poker-original-brancaazul-_JM#polycard_client=search-nordic&amp;position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Bwf15ab 15kg Tira Manchas Branca Brastemp Cor Branco 220V</t>
+          <t>Bola De Futebol Society 8 X Penalty</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>2211</v>
+        <v>154.71</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_901572-MLU74842910584_032024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_818310-MLU76366734942_052024-E.webp</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-bwf15ab-15kg-tira-manchas-branca-brastemp-cor-branco-220v/p/MLB27702613#polycard_client=search-nordic&amp;searchVariation=MLB27702613&amp;wid=MLB4119804368&amp;position=24&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-society-8-x-penalty/p/MLB19776132#polycard_client=search-nordic&amp;searchVariation=MLB19776132&amp;wid=MLB3829143887&amp;position=15&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Máquina De Lavar 15kg Electrolux Premium (lec15) Cor Branco 110V</t>
+          <t>Bola De Futebol Campo Uhlsport Match R1 Brasileirão 2025</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>2261</v>
+        <v>155.99</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_756379-MLU77364385393_072024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_857447-MLB82813326112_032025-E-bola-de-futebol-campo-uhlsport-match-r1-brasileiro-2025.webp</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-15kg-electrolux-premium-lec15-cor-branco-110v/p/MLB36579268#polycard_client=search-nordic&amp;searchVariation=MLB36579268&amp;wid=MLB5017435998&amp;position=15&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4003764129-bola-de-futebol-campo-uhlsport-match-r1-brasileiro-2025-_JM#polycard_client=search-nordic&amp;position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Máquina de Lavar Electrolux LEC15 Branca 15kg Premium Care com Cesto Inox Jet&amp;Clean e Time Control 220V</t>
+          <t>Bola De Campo Penalty S11 R2 Xxv ( Camp.paulista)</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>2261</v>
+        <v>159.9</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_607815-MLU77146379044_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_687100-MLB82940622023_032025-E-bola-de-campo-penalty-s11-r2-xxv-camppaulista.webp</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-electrolux-lec15-branca-15kg-premium-care-com-cesto-inox-jetclean-e-time-control-220v/p/MLB36731713#polycard_client=search-nordic&amp;searchVariation=MLB36731713&amp;wid=MLB5017447374&amp;position=47&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-3996246671-bola-de-campo-penalty-s11-r2-xxv-camppaulista-_JM?searchVariation=187147572233#polycard_client=search-nordic&amp;searchVariation=187147572233&amp;position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Lavadora Digital Inverter Samsung Ww11t Branca 11kg Cor Branco 110V</t>
+          <t>Bola Futebol De Campo Bola 8 Penalty Cor Preto</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>2359</v>
+        <v>164</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_763583-MLU78406525997_082024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_888107-MLA81942694869_012025-E.webp</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lavadora-digital-inverter-samsung-ww11t-branca-11kg-cor-branco-110v/p/MLB39327272#polycard_client=search-nordic&amp;searchVariation=MLB39327272&amp;wid=MLB3818670393&amp;position=50&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-de-campo-bola-8-penalty-cor-preto/p/MLB22210458#polycard_client=search-nordic&amp;searchVariation=MLB22210458&amp;wid=MLB3945165169&amp;position=37&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Brastemp 15kg Cinza Platinum Com Timer Pro 110V</t>
+          <t>Bola De Futebol Dalponte 81 Nitro Society Costurada À Mão Cor Branco</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>2439</v>
+        <v>176.62</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_735856-MLU76143998613_052024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_756582-MLU74393181908_022024-E.webp</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-brastemp-15kg-cinza-platinum-com-timer-pro-110v/p/MLB36504260#polycard_client=search-nordic&amp;searchVariation=MLB36504260&amp;wid=MLB3802426827&amp;position=38&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-dalponte-81-nitro-society-costurada-mo-cor-branco/p/MLB32946547#polycard_client=search-nordic&amp;searchVariation=MLB32946547&amp;wid=MLB3596272369&amp;position=21&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Led17 Branco Essential Care 17kg Electrolux</t>
+          <t>Bola Futebol Society 8 Pro Xxiv Tamanho 5 Cor Preto e Branco Penalty</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>2535</v>
+        <v>297</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_999868-MLA82370834951_022025-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_819669-MLU75482475121_032024-E.webp</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-led17-branco-essential-care-17kg-electrolux/p/MLB46017200#polycard_client=search-nordic&amp;searchVariation=MLB46017200&amp;wid=MLB5285022924&amp;position=51&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-society-8-pro-xxiv-tamanho-5-cor-preto-e-branco-penalty/p/MLB35142675#polycard_client=search-nordic&amp;searchVariation=MLB35142675&amp;wid=MLB4630087278&amp;position=14&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Máquina De Lavar Brastemp 17kg Branca - Bwk17ab Cor Branco 220V</t>
+          <t>Bola De Futsal Penalty Max 1000 Xxiv Cor Azul</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>2577</v>
+        <v>298.28</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_935520-MLU77119876248_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_973308-MLU75866936168_042024-E.webp</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/maquina-de-lavar-brastemp-17kg-branca-bwk17ab-cor-branco-220v/p/MLB22636409#polycard_client=search-nordic&amp;searchVariation=MLB22636409&amp;wid=MLB5152699940&amp;position=52&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-penalty-max-1000-xxiv-cor-azul/p/MLB36227619#polycard_client=search-nordic&amp;searchVariation=MLB36227619&amp;wid=MLB3937932227&amp;position=25&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Lava E Seca Midea Master Clean Smart 11kg Branca 127v</t>
+          <t>Bola Uhlsport Campo Game Pro Brasileirão Série C E D 2025</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>3195</v>
+        <v>379</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_730553-MLU77374801689_072024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_652481-MLB82865558482_032025-E-bola-uhlsport-campo-game-pro-brasileiro-serie-c-e-d-2025.webp</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lava-e-seca-midea-master-clean-smart-11kg-branca-127v/p/MLB37296614#polycard_client=search-nordic&amp;searchVariation=MLB37296614&amp;wid=MLB5178870222&amp;position=26&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4006258699-bola-uhlsport-campo-game-pro-brasileiro-serie-c-e-d-2025-_JM?searchVariation=187252357205#polycard_client=search-nordic&amp;searchVariation=187252357205&amp;position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Lava e seca Midea Master Clean Smart 11kg Titanium Mfm01d110wb/tkbr04 127v</t>
+          <t>Kit 50 Bolas Futebol Couro Sintético Costurada N°05</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>3299</v>
+        <v>916</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_979698-MLU77125322082_062024-V.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_871334-MLB82990085837_032025-E-kit-50-bolas-futebol-couro-sintetico-costurada-n05.webp</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/lava-e-seca-midea-master-clean-smart-11kg-titanium-mfm01d110wbtkbr04-127v/p/MLB37448773#polycard_client=search-nordic&amp;searchVariation=MLB37448773&amp;wid=MLB3909021837&amp;position=6&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Lava e Seca Midea MF200D110WB 11Kg Midea HealthGuard Titanium Conectada 127V</t>
-        </is>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>3427</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_927592-MLU76537680465_052024-V.webp</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>https://www.mercadolivre.com.br/lava-e-seca-midea-mf200d110wb-11kg-midea-healthguard-titanium-conectada-127v/p/MLB19136202#polycard_client=search-nordic&amp;searchVariation=MLB19136202&amp;wid=MLB3775715141&amp;position=14&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Lava e Seca Midea MF200D110WB 11Kg HealthGuard Titanium Conectada 220v</t>
-        </is>
-      </c>
-      <c r="B53" s="2" t="n">
-        <v>3427</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_842109-MLU72566235196_112023-V.webp</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>https://www.mercadolivre.com.br/lava-e-seca-midea-mf200d110wb-11kg-healthguard-titanium-conectada-220v/p/MLB19136205#polycard_client=search-nordic&amp;searchVariation=MLB19136205&amp;wid=MLB3775715131&amp;position=12&amp;search_layout=stack&amp;type=product&amp;tracking_id=3ee44d1b-ae16-41f8-9e78-c77081a73b22&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-5313103164-kit-50-bolas-futebol-couro-sintetico-costurada-n05-_JM?searchVariation=183096595076#polycard_client=search-nordic&amp;searchVariation=183096595076&amp;position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add 'loading', fix chromedriver, fix find_elements
</commit_message>
<xml_diff>
--- a/produtos_ordenados.xlsx
+++ b/produtos_ordenados.xlsx
@@ -469,7 +469,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>12.81</v>
+        <v>21.65</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -478,594 +478,594 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/saco-para-ate-10-bolas-porta-bolas-fio-4mm-branco/p/MLB25996601#polycard_client=search-nordic&amp;searchVariation=MLB25996601&amp;wid=MLB4147585512&amp;position=5&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/saco-para-ate-10-bolas-porta-bolas-fio-4mm-branco/p/MLB25996601?searchVariation=MLB25996601#polycard_client=search-nordic&amp;searchVariation=MLB25996601&amp;wid=MLB3489017277&amp;position=21&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bola De Futebol Para Campo Tamanho 5 Petrin Presente Cor</t>
+          <t>Bola Infantil Escolar Queimada T10 Vollo Iniciação Esportiva Cor Laranja</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>18.37</v>
+        <v>36.92</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_859381-MLA81212900247_122024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_878434-MLB51582630730_092022-E.webp</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-para-campo-tamanho-5-petrin-presente-cor/p/MLB44556814#polycard_client=search-nordic&amp;searchVariation=MLB44556814&amp;wid=MLB4007228671&amp;position=39&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-infantil-escolar-queimada-t10-vollo-iniciaco-esportiva-cor-laranja/p/MLB19718998?searchVariation=MLB19718998#polycard_client=search-nordic&amp;searchVariation=MLB19718998&amp;wid=MLB2940254386&amp;position=39&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Trave Futebol Gol Kit Mini Golzinho Infantil Brinquedo Bola</t>
+          <t>Bola Iniciação De Borracha 12 Magussy Cor Verde</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>33.54</v>
+        <v>38.9</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_764435-MLA79889067517_102024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_854080-MLB31117752008_062019-E.webp</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/trave-futebol-gol-kit-mini-golzinho-infantil-brinquedo-bola/p/MLB41775954#polycard_client=search-nordic&amp;searchVariation=MLB41775954&amp;wid=MLB5118193404&amp;position=11&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-iniciaco-de-borracha-12-magussy-cor-verde/p/MLB20578581?searchVariation=MLB20578581#polycard_client=search-nordic&amp;searchVariation=MLB20578581&amp;wid=MLB3079846120&amp;position=22&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tabela De Medição De Pressão, Medidor De Ponteiro De Futebol</t>
+          <t>Bola Futebol Queimada Iniciação De Borracha 14 Magussy Cor Laranja</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>38.31</v>
+        <v>43.5</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_725638-CBT81594394892_012025-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_907909-MLB42249022185_062020-E.webp</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/pressure-measurement-table-portable-football-pointer-gauge/p/MLB2009472856#polycard_client=search-nordic&amp;searchVariation=MLB2009472856&amp;wid=MLB4000139541&amp;position=9&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-queimada-iniciaco-de-borracha-14-magussy-cor-laranja/p/MLB22313946?searchVariation=MLB22313946#polycard_client=search-nordic&amp;searchVariation=MLB22313946&amp;wid=MLB3409769135&amp;position=18&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bola Futebol Tamanho 5 Capotão + Bomba De Ar E Bico Cor Azul</t>
+          <t>Bola De Futsal Sandrini Strike Pro Oficial Alta Performance</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>39.99</v>
+        <v>49.58</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_628564-MLU78026959026_082024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_853272-MLB83998028405_042025-E-bola-de-futsal-sandrini-strike-pro-oficial-alta-performance.webp</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-futebol-tamanho-5-capoto-bomba-de-ar-e-bico-cor-azul/p/MLB39157733#polycard_client=search-nordic&amp;searchVariation=MLB39157733&amp;wid=MLB3870171799&amp;position=30&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=yFY0NMfIaBac5HMHB%2Fm3ln6SBTS%2BBbkMb5m8dDJHYYxNtiu9JYhED9fjlhQLDMlCd7URHt0g10ZJLlucFpNU0wgOdely6tKw01%2Bp8XrXyQfHdb3boJ1Q8SmvnpcWBjX3TizitpnJm4nZJJNTw0UfB2ZOJmaOCg%2B4yB2amrm%2BHZTJ3TI1oCQeoXvO0R2wgcpgF46i7xcbV870eUc319etjml%2F6ejxQU1epBt%2BM8OQzgHpxQaZoi%2FsHQfCIM0idyze7zGYAAJyhoLtVN7%2B8hPFaL0ekLhvSUrnnEOdtPvcBSdS2MFXVfGjSUYcIRa8Pd2jD0s1dVfKxT1kM9Tgma3vzlgAMHVZ%2F%2BwAhBuvckmPSMRuT1D4PDOk3nXDV%2BFZROI4P2frfVCKZLMwWlZINW%2BswoY%2BZTxFw3hqcoCkZ6KoAuilMkPHPaporJDr3VTpa5Mf7MIXD%2FzlloxOR9uFDrkTzdFmn%2B1bRJrS1%2FFnjOud0qnKQQt9RH1ydJrYUf6rkeZaoG38NucQmX%2FTaBNDTx5gsYGpfQKwqa%2B4R7IRRQzdj4rvH%2FvI1MC%2FbZKx3NUkJ%2BeNkgwYzbV9ItbA1IwPUVsZcnU6fq%2BJ54gDgw8PmrhapJ%2BrK3GVRL99rDd61pBfcaFzz3lg7QvbIY1RsMVHlw3Ihr4CNuinIrznyMEDYJVYas6N3PYofB7ERVwoGe4rAXkj7jtdQHNly5a42rKsJ0RpaoS1REoRt1ubXnt0WfsiVxYl9NFdWidFtA2hBlmK6Z%2F7kedw1IhMR90FOa%2BGBwUunSgyh68PP5pu%2FiH44oikk0tyBzaUEE22Ek%2BbKkd8%2Fn6VYBlr6VN5hy7D45dXed0OvP3EiBvLcNNDUx4H9sxWvouMO4gucf%2B5WD7qBD4%3D&amp;searchVariation=187629540185#polycard_client=search-nordic&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kit Bola De Vôlei + Bola De Futebol + Bomba Pró Sortidas</t>
+          <t>Bola De Futsal Sandrini Strike Pro Oficial Alta Performance</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>41.22</v>
+        <v>49.58</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_702577-MLA82266657438_022025-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_853272-MLB83998028405_042025-E-bola-de-futsal-sandrini-strike-pro-oficial-alta-performance.webp</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/kit-bola-de-vlei-bola-de-futebol-bomba-pro-sortidas/p/MLB46184165#polycard_client=search-nordic&amp;searchVariation=MLB46184165&amp;wid=MLB5292902016&amp;position=22&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4040460061-bola-de-futsal-sandrini-strike-pro-oficial-alta-performance-_JM?searchVariation=187629540185#polycard_client=search-nordic&amp;searchVariation=187629540185&amp;position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bola De Vôlei 3.5 Texturizada Amarela Rainha Topper</t>
+          <t>Bola Iniciação De Borracha T12 Penalty Iniciação Crianças Cor Azul</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44.99</v>
+        <v>52.9</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_875461-MLU78119836106_082024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_631736-MLB52523687277_112022-E.webp</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-vlei-35-texturizada-amarela-rainha-topper/p/MLB21012198#polycard_client=search-nordic&amp;searchVariation=MLB21012198&amp;wid=MLB3963193225&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-iniciaco-de-borracha-t12-penalty-iniciaco-criancas-cor-azul/p/MLB21906104?searchVariation=MLB21906104#polycard_client=search-nordic&amp;searchVariation=MLB21906104&amp;wid=MLB5348589720&amp;position=8&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bola De Futebol Luke Sports Tamanho 5 Campo E Society Branca Cor Branco</t>
+          <t>A+ Futebol De Treinamento Euro 5 2024</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>48.29</v>
+        <v>55.74</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_921199-MLA80927520322_122024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_893064-MLB84246921498_052025-E.webp</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-luke-sports-tamanho-5-campo-e-society-branca-cor-branco/p/MLB44516604#polycard_client=search-nordic&amp;searchVariation=MLB44516604&amp;wid=MLB5214268684&amp;position=32&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/entrenamiento-de-futbol-euro5-2024/p/MLB2017321288#polycard_client=search-nordic&amp;searchVariation=MLB2017321288&amp;wid=MLB4058260225&amp;position=32&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>10 Bolas De Vinil Futebol Dente De Leite C/ Cor Branco Com Preto</t>
+          <t>Bola De Futsal Slick 22 Topper Cor Branco/Amarelo Neon/Azul</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>48.97</v>
+        <v>62.23</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_785671-MLU77640619462_072024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_656329-MLB54078855245_022023-E.webp</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/10-bolas-de-vinil-futebol-dente-de-leite-c-cor-branco-com-preto/p/MLB38350019#polycard_client=search-nordic&amp;searchVariation=MLB38350019&amp;wid=MLB3855446145&amp;position=24&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-22-topper-cor-brancoamarelo-neonazul/p/MLB22262771?searchVariation=MLB22262771#polycard_client=search-nordic&amp;searchVariation=MLB22262771&amp;wid=MLB3820042822&amp;position=29&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Bola De Futebol De Campo Slick 2020 Topper Cor Amarelo Neon/Preto</t>
+          <t>Bola De Futebol Society Slick 2020 Cor Branco/Preto/Amarelo Tamanho Único Topper</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>48.99</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_969183-MLU75988202853_042024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_869053-MLB51937100243_102022-E.webp</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-slick-2020-topper-cor-amarelo-neonpreto/p/MLB19754376#polycard_client=search-nordic&amp;searchVariation=MLB19754376&amp;wid=MLB5277328830&amp;position=38&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-society-slick-2020-cor-brancopretoamarelo-tamanho-unico-topper/p/MLB19744266?searchVariation=MLB19744266#polycard_client=search-nordic&amp;searchVariation=MLB19744266&amp;wid=MLB5222132312&amp;position=16&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bola De Futebol Slick Campo Cor Azul/Branco/Preto Topper</t>
+          <t>Bola De Futevôlei Diadora Elite-r Cor Amarelo</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>50.72</v>
+        <v>67.13</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_979047-MLU71168535619_082023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_699842-MLU70081962810_062023-E.webp</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-slick-campo-cor-azulbrancopreto-topper/p/MLB19765484#polycard_client=search-nordic&amp;searchVariation=MLB19765484&amp;wid=MLB5270990860&amp;position=35&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevlei-diadora-elite-r-cor-amarelo/p/MLB21096382?searchVariation=MLB21096382#polycard_client=search-nordic&amp;searchVariation=MLB21096382&amp;wid=MLB3383487155&amp;position=5&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Bola Futebol Society Ótimo Custo Beneficio Peso Ideal Top Cor Azul</t>
+          <t>Bola Futevolei Protech Diadora Elite-r Cor Branco</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>53.82</v>
+        <v>67.13</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_862896-MLU69453002841_052023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_645165-MLU78631385474_092024-E.webp</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-futebol-society-otimo-custo-beneficio-peso-ideal-top-cor-azul/p/MLB23339357#polycard_client=search-nordic&amp;searchVariation=MLB23339357&amp;wid=MLB3923038695&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futevolei-protech-diadora-elite-r-cor-branco/p/MLB39111515?searchVariation=MLB39111515#polycard_client=search-nordic&amp;searchVariation=MLB39111515&amp;wid=MLB3809247007&amp;position=34&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Bola De Futebol de Campo Slick 24 Tecnofusion Multicor Topper</t>
+          <t>Bola De Futebol Uhlsport Score Society Laranja</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>53.99</v>
+        <v>67.72</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_722050-MLU76926100481_062024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_776421-MLA83745761947_042025-E.webp</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-slick-24-tecnofusion-multicor-topper/p/MLB35378541#polycard_client=search-nordic&amp;searchVariation=MLB35378541&amp;wid=MLB3963108755&amp;position=40&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-uhlsport-score-society-laranja/p/MLB48256018?searchVariation=MLB48256018#polycard_client=search-nordic&amp;searchVariation=MLB48256018&amp;wid=MLB4055108227&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bola De Futebol De Campo Slick 2020 Topper</t>
+          <t>Bola De Futebol Para Campo 22 I Topper Cor Branco/Verde Mar/Preto</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>54.99</v>
+        <v>68.84999999999999</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_735756-MLB54078855256_022023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_967540-MLU69495823375_052023-E.webp</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-slick-2020-topper/p/MLB22262774#polycard_client=search-nordic&amp;searchVariation=MLB22262774&amp;wid=MLB5270990842&amp;position=13&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-para-campo-22-i-topper-cor-brancoverde-marpreto/p/MLB22272252?searchVariation=MLB22272252#polycard_client=search-nordic&amp;searchVariation=MLB22272252&amp;wid=MLB4198884500&amp;position=14&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bola De Futsal Slick 24 Câmara Airvility 6 Gomos Topper</t>
+          <t>Bola De Futsal Kagiva Slick  Sub 11</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>54.99</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_790020-MLU75616505649_042024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_908540-MLB84342735079_052025-E-bola-de-futsal-kagiva-slick-sub-11.webp</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-24-cmara-airvility-6-gomos-topper/p/MLB35378564#polycard_client=search-nordic&amp;searchVariation=MLB35378564&amp;wid=MLB3963063089&amp;position=29&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4052328075-bola-de-futsal-kagiva-slick-sub-11-_JM?searchVariation=187815505187#polycard_client=search-nordic&amp;searchVariation=187815505187&amp;position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bola De Futebol Para Campo 22 I Topper Cor Branco/Verde Mar/Preto</t>
+          <t>Topper Futsal Slick Bola Futebol Salão Branco Com Azul</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>55.85</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_967540-MLU69495823375_052023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_880504-MLU71134471481_082023-E.webp</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-para-campo-22-i-topper-cor-brancoverde-marpreto/p/MLB22272252#polycard_client=search-nordic&amp;searchVariation=MLB22272252&amp;wid=MLB4198884500&amp;position=4&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/topper-futsal-slick-bola-futebol-salo-branco-com-azul/p/MLB26148855?searchVariation=MLB26148855#polycard_client=search-nordic&amp;searchVariation=MLB26148855&amp;wid=MLB4703197748&amp;position=15&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bola De Futebol Campo Slick Cup Topper</t>
+          <t>Bola De Futebol Slick Campo Cor Azul/Branco/Preto Topper</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>59.15</v>
+        <v>69.11</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_659913-MLA80298884457_102024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_979047-MLU71168535619_082023-E.webp</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-campo-slick-cup-topper/p/MLB19698380#polycard_client=search-nordic&amp;searchVariation=MLB19698380&amp;wid=MLB5189140588&amp;position=8&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-slick-campo-cor-azulbrancopreto-topper/p/MLB19765484?searchVariation=MLB19765484#polycard_client=search-nordic&amp;searchVariation=MLB19765484&amp;wid=MLB3784862677&amp;position=10&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bola De Futsal Slick 22 Topper Cor Branco/Amarelo Neon/Azul</t>
+          <t>Bola Futebol Society Ótimo Custo Beneficio Peso Ideal Top Cor Azul</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>59.2</v>
+        <v>69.11</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_656329-MLB54078855245_022023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_822484-MLA84472440243_052025-E.webp</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-22-topper-cor-brancoamarelo-neonazul/p/MLB22262771#polycard_client=search-nordic&amp;searchVariation=MLB22262771&amp;wid=MLB3820042822&amp;position=12&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-society-otimo-custo-beneficio-peso-ideal-top-cor-azul/p/MLB23339357?searchVariation=MLB23339357#polycard_client=search-nordic&amp;searchVariation=MLB23339357&amp;wid=MLB5105345848&amp;position=9&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Bola De Futsal Slick Cup Topper Cor Laranja/Azul Anodizado/Preto</t>
+          <t>Bola De Futebol Licenciada Corinthians (sccp) N° 5 Cor Preto</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>59.9</v>
+        <v>77.88</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_882043-MLU75981819389_042024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_836019-MLU78000914804_082024-E.webp</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futsal-slick-cup-topper-cor-laranjaazul-anodizadopreto/p/MLB19710248#polycard_client=search-nordic&amp;searchVariation=MLB19710248&amp;wid=MLB2889188605&amp;position=36&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-licenciada-corinthians-sccp-n-5-cor-preto/p/MLB39115009?searchVariation=MLB39115009#polycard_client=search-nordic&amp;searchVariation=MLB39115009&amp;wid=MLB3956648899&amp;position=43&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Topper Futsal Slick Bola Futebol Salão Branco Com Azul</t>
+          <t>Bola Futevolei Altinha Rio Vulcanizada Fut Mesa Luke Sports Cor Amarelo</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>60.99</v>
+        <v>77.98999999999999</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_880504-MLU71134471481_082023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_896782-MLU72643073783_112023-E.webp</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/topper-futsal-slick-bola-futebol-salo-branco-com-azul/p/MLB26148855#polycard_client=search-nordic&amp;searchVariation=MLB26148855&amp;wid=MLB3963093661&amp;position=17&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futevolei-altinha-rio-vulcanizada-fut-mesa-luke-sports-cor-amarelo/p/MLB21418949?searchVariation=MLB21418949#polycard_client=search-nordic&amp;searchVariation=MLB21418949&amp;wid=MLB4035567809&amp;position=13&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bola De Futebol Society Slick 2020 Cor Branco/Preto/Amarelo Tamanho Único Topper</t>
+          <t>Bola Futevolei Altinha Rio Vulcanizada Fut Mesa Luke Sports Cor Branco</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>61.76</v>
+        <v>77.98999999999999</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_869053-MLB51937100243_102022-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_969914-MLA53311863193_012023-E.webp</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-society-slick-2020-cor-brancopretoamarelo-tamanho-unico-topper/p/MLB19744266#polycard_client=search-nordic&amp;searchVariation=MLB19744266&amp;wid=MLB5222132312&amp;position=20&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futevolei-altinha-rio-vulcanizada-fut-mesa-luke-sports-cor-branco/p/MLB21740597?searchVariation=MLB21740597#polycard_client=search-nordic&amp;searchVariation=MLB21740597&amp;wid=MLB4035606743&amp;position=17&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Bola De Futevolei Altinha N°5 Quadra Areia Pro Praia</t>
+          <t>Bola Campo Kappa Blasty</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>65.97</v>
+        <v>78.90000000000001</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_645076-MLB82458925554_022025-E-bola-de-futevolei-altinha-n5-quadra-areia-pro-praia.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_647523-MLB83740061954_042025-E-bola-campo-kappa-blasty.webp</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=mYpbkfZv%2BWrkHXFcJzH%2BLNwYdTR0CClKwqUNkB8gCyWC%2FkdDlw6z8okZwVrmsuyR2mvs0GYH0ptERW22b6tFsUz0f5KJyKt0nZlkml5NHIihom1Px0J1CrbZ6BSH%2FQTGQE6B9ax%2B8GkDXee%2B3gEdsQRcITpBPk4s%2Fw8gpWzkpb6nHYDnDCDl2xtI3hK1lB3Wd5%2F%2Fd%2F80G3ATney9LcSZw2H4xE2MA85NvXkt7eZqjfydIIsRHfEjNqfi%2FkCWbCW44xypAzY70XuE9F34Sb0BBB5IrTcC1McHT%2FQt4QIlLn5MravpRWVd4SjFa6QU9%2FCOQJCek3J%2BfhFmi6pNVPwdjvRnCYAj5w617jbLWvuC9BJT0I8D7bMaV8QDGZALYfTZOfGT97MfuUXaR8ghh0ObguNGxU55WI2FSBFhZdflUaZsCNlQoxpEcAePwzEG3z85QfUHPHfZqR5w0na0JYqMbdr4SD8yNvtmACVwSDGRi44oCy3mDQxN6SD%2B0ksm4DoC%2BV3xPf2OEQcAkZByaZrXT4%2B3gafEjiieOk%2FK3hq79iySWUkvbfQ9s%2FKjQRQuB2SFp7BdKa3JXs9ckJwlOhqDwF9W6qK6NtExi5tDMVlig4EIBE85sqQAg46ddNkNlAHoWDGbafgKjwSTAxNppif8QmfMEE%2B26ocAjnPEHS8rDpgCfzEUyAQrou8F0S38ZvEluacn6hROTtflt0mPDQE7axmgsZnO2W9VsgeQreDZnbUF1SNZwEQeM11LfwQqyyGH%2Bme8eNvc8LGIA8UlFpcKtslbO%2FoJPAGu4A%2B0tShxXMRtpBbPDC9usKwaFGuPT7W5MhE6hmd3jfwtV84NEsMGcnY5tzYenexutjdg&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4041791677-bola-campo-kappa-blasty-_JM?searchVariation=187650319665#polycard_client=search-nordic&amp;searchVariation=187650319665&amp;position=50&amp;search_layout=grid&amp;type=item&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bola De Futevolei Altinha N°5 Quadra Areia Pro Praia</t>
+          <t>Bola Futsal Penalty Rx 500 Xxiii Cor Azul</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>65.97</v>
+        <v>78.98999999999999</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_645076-MLB82458925554_022025-E-bola-de-futevolei-altinha-n5-quadra-areia-pro-praia.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_722195-MLU77108763060_062024-E.webp</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-4006687617-bola-de-futevolei-altinha-n5-quadra-areia-pro-praia-_JM?searchVariation=183156389516#polycard_client=search-nordic&amp;searchVariation=183156389516&amp;position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-futsal-penalty-rx-500-xxiii-cor-azul/p/MLB25820360?searchVariation=MLB25820360#polycard_client=search-nordic&amp;searchVariation=MLB25820360&amp;wid=MLB3954480337&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Bola De Futevôlei Diadora Elite-r</t>
+          <t>Bola De Futsal Rx 500 Xxiii Cor Branco Amarelo E Preto Penalty</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>69.59999999999999</v>
+        <v>84.12</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_777673-MLB74305800482_022024-E-bola-de-futevlei-diadora-elite-r.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_750391-MLA72526096144_102023-E.webp</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=FA2v80kO0Q62jIC3APOe8OLdHZosDSTo1hLLRyRzr90a4JOmG9fNJuYmnoO8wg22iqTmr27d%2BrK3sZOAMDcUxTXULya%2FuqG3Uce7FwirY265ddOp%2FaRo0%2FUfe1%2Fe8RReqaCkhX4gJYzGKk62Jq9YuTkU%2FZbzoSwUeYEBMevSBPog0Bu0gIxXMJ93cIk4gUOvWjnzprMXLSMEiSakhNXOETkZc5KUFk1bQXqKVFLpHWMuz2XLh68FPbRohnW7tl%2BCcmfgQvwQKhoklCxqKO8wcN%2B12x61YphpgBIMTsCsHnlUsyjm18ZhifBDehyGu9uKFLf5gpt612eYaSwpb3psZ42tp7JY20HPiQBPpcWki4%2FqHPJIE8iZwN9PD8PRPxmFi%2B%2F9jhfUYSfXKW7I6emq3gWPDPAro%2BtAPq1Mlbu1WvjcEOFDOeYK%2F4o56stlpSmFH4zTluHTF8HsKZqH49c8i6VjRDwLf4JiWGWPeyy5JuASJg7cJfmPAASSftaG%2B5b%2BFAQx5qMBbAgkFrIVkMakbpJyEXx8LKisH3WrSN3mVVhT%2Bal25Bev9FVuqCIkH5rpVvnIOIthHtGurHdG5%2FUMhpGuYitAJxoXDha%2FceYFueTm8Ya0XdxcZd4LtZXVUsnvCxj%2FjN%2B5R%2BqrYb4uyMOPasbyNJqMjg4nxO6hb6fRGkW5imtNH17dsnmSd22hBtwdRfUtVo6b7VeYEEiD72oR%2Bf2sqpC8IVbMa%2B5uV03kiM3O7Atg3Dc6%2FLHKx%2Blem1khGGw4rvQ51VV%2FLhtFT0uDGeA367TVDZlCRBGdGq%2F8EF4H0r0oG9GbdOGxqt7Ld0bygm%2FBhLfnOQ%3D%3D&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-rx-500-xxiii-cor-branco-amarelo-e-preto-penalty/p/MLB22341158?searchVariation=MLB22341158#polycard_client=search-nordic&amp;searchVariation=MLB22341158&amp;wid=MLB3497005067&amp;position=11&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bola De Futevôlei Diadora Elite-r</t>
+          <t>Bola Futsal Penalty Rx 200 Xxiii - Tamanho Único Cor Amarelo</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>69.59999999999999</v>
+        <v>88.86</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_777673-MLB74305800482_022024-E-bola-de-futevlei-diadora-elite-r.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_924774-MLU74087035735_012024-E.webp</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3705513048-bola-de-futevlei-diadora-elite-r-_JM?searchVariation=177953619994#polycard_client=search-nordic&amp;searchVariation=177953619994&amp;position=50&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-futsal-penalty-rx-200-xxiii-tamanho-unico-cor-amarelo/p/MLB24090041?searchVariation=MLB24090041#polycard_client=search-nordic&amp;searchVariation=MLB24090041&amp;wid=MLB3632679633&amp;position=26&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bola De Futevôlei Diadora Elite-r Cor Amarelo</t>
+          <t>Bolas De Futebol Tamanho 5 Team Match Group Training Pvc Hig</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>74.92</v>
+        <v>92.25</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_699842-MLU70081962810_062023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_941067-CBT84265222412_052025-E.webp</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futevlei-diadora-elite-r-cor-amarelo/p/MLB21096382#polycard_client=search-nordic&amp;searchVariation=MLB21096382&amp;wid=MLB3383487155&amp;position=19&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/size-5-soccer-balls-team-match-group-training-pvc-high-quali/p/MLB2017854866#polycard_client=search-nordic&amp;searchVariation=MLB2017854866&amp;wid=MLB4058867027&amp;position=40&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bola De Campo Topper Slick Gold Dourada Oficial Bomba De Ar</t>
+          <t>Bola Starlancer Club adidas Cor Blue / White</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>74.95</v>
+        <v>93.16</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_869593-MLB82719894389_022025-E-bola-de-campo-topper-slick-gold-dourada-oficial-bomba-de-ar.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_653697-MLA79844507542_102024-E.webp</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3987100373-bola-de-campo-topper-slick-gold-dourada-oficial-bomba-de-ar-_JM?searchVariation=183000579442#polycard_client=search-nordic&amp;searchVariation=183000579442&amp;position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-starlancer-club-adidas-cor-blue-white/p/MLB32495473?searchVariation=MLB32495473#polycard_client=search-nordic&amp;searchVariation=MLB32495473&amp;wid=MLB5122408382&amp;position=19&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Bola Para Futebol De Campo Bravo Xxiv Branco e Azul Penalty</t>
+          <t>Conjunto De Guirlandas De Balões De Decoração De Morango Str</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>77.90000000000001</v>
+        <v>96.56</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_698520-MLU75981724023_042024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_975428-CBT84563384451_052025-E.webp</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-para-futebol-de-campo-bravo-xxiv-branco-e-azul-penalty/p/MLB27895686#polycard_client=search-nordic&amp;searchVariation=MLB27895686&amp;wid=MLB3951567371&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/trawberry-gathering-decoration-balloon-garland-set-strawberr/p/MLB2017423693#polycard_client=search-nordic&amp;searchVariation=MLB2017423693&amp;wid=MLB4058639209&amp;position=36&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Bola Futsal Penalty Rx 500 Xxiii Cor Azul</t>
+          <t>Bola Futebol De Campo Topper Slick 22 Oficial + Bomba De Ar</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>78.90000000000001</v>
+        <v>97.63</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_722195-MLU77108763060_062024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_732799-MLB74418884230_022024-E-bola-futebol-de-campo-topper-slick-22-oficial-bomba-de-ar.webp</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-futsal-penalty-rx-500-xxiii-cor-azul/p/MLB25820360#polycard_client=search-nordic&amp;searchVariation=MLB25820360&amp;wid=MLB3996965885&amp;position=16&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=sw6uyYhc3hvfNFUV1ejBrq2tXIwUeasI5mxwjRmJWVc4ySkcLEDbuubv%2BXJsyuu5qf6o7cJNtgOqJcOepGZoFooUT%2BTIJSPcJFa%2F0d50NIABDAX%2BOqKyMi%2F5jboz3on4ONPxziMUdm1TdJ8MEfJvfZFccubWdGa5BHPS7xbJYiCciMa0D7zXQdzdMz29ZNpwXWmX3wen7HU5JdWJayefOMbewUj6WlFcOlp3GlW9mH5eaTRIywTJfuOu9C67254Kc%2FPjaLFg64H7GhWLnSwdAdu8nPno7P4OEThUlEkuriOypj3xg%2BCo9AmmRVb2%2Bwn2e0EP1UE05O603%2FqQ8MihmnXNWTp5vkDQPLy6mf6X9c7B25rhkYHc3KoWbacDy6%2FgcqbCXH3nSEmZJIPhbT61IF7512vVVO0hhTQhFLm%2FqiDDRfPlaww9mjXnDAzDPEn2BN2fXR1YfI%2B1TwT43ttowkkBDUV0w4qW031gIc21URKeDJ2cO%2BK1GXthWPztXSI3vL3oCmc0915P%2BUA9U7o%2Fd8jTgBkcMlUKo4OWD0xVxdgVt7E6l%2FSQKsX3XJWRBQdUAo6cRoeniayTwQVeJW%2FMt0e8CODC14wA%2BiVCOpSRb0DA7F4rUvHhbGlAZXd0ZdBqJUTUWIa8t3cX8WOlnuAeq2aIQR8ZtkX0TMKk0irXQfhHNueTRyNte1aWTxZW3%2FojfnkQYCqGN8NQ%2F8KkHo%2BgJEH9jTUoAtxZG3dTCuCGqREEIdreVqmnWMOqC8avcm5orCV%2BO6KDDmFWZZh%2FbbiKd5UMcE9kl%2B4BvlTi4QtExbti%2BrEdQ15cnd6fbZ19wqlUzA%2BgN2gyD1qqMn%2FtFl0DVw5AIb46FwbC7zmYVjZH4wn%2BEow0o3wEhT0%3D&amp;searchVariation=177634599863#polycard_client=search-nordic&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Bola De Futebol Branco E Laranja De Campo Bravo Xxiv Penalty</t>
+          <t>Bola Futebol De Campo Topper Slick 22 Oficial + Bomba De Ar</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>78.98999999999999</v>
+        <v>97.63</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_764251-MLU75813169222_042024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_732799-MLB74418884230_022024-E-bola-futebol-de-campo-topper-slick-22-oficial-bomba-de-ar.webp</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-branco-e-laranja-de-campo-bravo-xxiv-penalty/p/MLB27893082#polycard_client=search-nordic&amp;searchVariation=MLB27893082&amp;wid=MLB5056295770&amp;position=23&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-3283893849-bola-futebol-de-campo-topper-slick-22-oficial-bomba-de-ar-_JM?searchVariation=177634599863#polycard_client=search-nordic&amp;searchVariation=177634599863&amp;position=49&amp;search_layout=grid&amp;type=item&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bola Para Futebol De Campo Líder Xxiv Cor Branco/Azul/Verde Penalty</t>
+          <t>Bola adidas Starlancer Jh3748 Tamanho 5</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
@@ -1073,172 +1073,172 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_895518-MLU74287171999_012024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_700816-MLA80927391270_122024-E.webp</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-para-futebol-de-campo-lider-xxiv-cor-brancoazulverde-penalty/p/MLB30924589#polycard_client=search-nordic&amp;searchVariation=MLB30924589&amp;wid=MLB3937962097&amp;position=10&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-adidas-starlancer-jh3748-tamanho-5/p/MLB44513782?searchVariation=MLB44513782#polycard_client=search-nordic&amp;searchVariation=MLB44513782&amp;wid=MLB3996195869&amp;position=28&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bola Allpha Futsal Pró+ Madri Pu Maciez Treino Original</t>
+          <t>Cabo De Freio 133-8158 Para Cortador De Grama Timemaster De</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>106.69</v>
+        <v>105.46</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_965545-MLB82741758954_032025-E-bola-allpha-futsal-pro-madri-pu-maciez-treino-original.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_760371-CBT84265591818_052025-E.webp</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-4000309717-bola-allpha-futsal-pro-madri-pu-maciez-treino-original-_JM?searchVariation=183112590022#polycard_client=search-nordic&amp;searchVariation=183112590022&amp;position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/133-8158-brake-cable-for-toro-30inch-timemaster-lawn-mower/p/MLB2017418961#polycard_client=search-nordic&amp;searchVariation=MLB2017418961&amp;wid=MLB4058727039&amp;position=35&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Bola de Futebol Penalty Society Lider XXIV Branco Laranja Azul 5</t>
+          <t>Penalty Bola Campo S11 R2 Xxv</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>111.71</v>
+        <v>111.84</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_903645-MLU74833063908_032024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_809583-MLA82638539265_022025-E.webp</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-penalty-society-lider-xxiv-branco-laranja-azul-5/p/MLB27892495#polycard_client=search-nordic&amp;searchVariation=MLB27892495&amp;wid=MLB3951591553&amp;position=18&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/penalty-bola-campo-s11-r2-xxv/p/MLB45335231?searchVariation=MLB45335231#polycard_client=search-nordic&amp;searchVariation=MLB45335231&amp;wid=MLB3957681981&amp;position=23&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Bola Society Líder Xxiv Pu Laminado 6 Gomos Penalty</t>
+          <t>Penalty Bola Society S11 R2 Xxv</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>114.99</v>
+        <v>120</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_609551-MLU78177695411_082024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_909398-MLA81733802801_012025-E.webp</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-society-lider-xxiv-pu-laminado-6-gomos-penalty/p/MLB27924191#polycard_client=search-nordic&amp;searchVariation=MLB27924191&amp;wid=MLB3938335813&amp;position=7&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/penalty-bola-society-s11-r2-xxv/p/MLB45246763?searchVariation=MLB45246763#polycard_client=search-nordic&amp;searchVariation=MLB45246763&amp;wid=MLB3957630395&amp;position=38&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Bola De Futebol Corinthians Time Oficial Licenciada Timão</t>
+          <t>Bola De Futebol De Campo Líder Xxiv Tamanho 5 Penalty</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>119</v>
+        <v>124.9</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_707361-MLB82839791767_032025-E-bola-de-futebol-corinthians-time-oficial-licenciada-timo.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_820448-MLU74857870237_032024-E.webp</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3992563623-bola-de-futebol-corinthians-time-oficial-licenciada-timo-_JM?searchVariation=187103662249#polycard_client=search-nordic&amp;searchVariation=187103662249&amp;position=49&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-de-campo-lider-xxiv-tamanho-5-penalty/p/MLB28612487?searchVariation=MLB28612487#polycard_client=search-nordic&amp;searchVariation=MLB28612487&amp;wid=MLB4397815064&amp;position=42&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bola Futevolei Altinha Ftv Ft5 Penta Futemesa Rio Cor Preto</t>
+          <t>Bola 81 Dalponte Star Campo Costurada A Mão Original</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>126.85</v>
+        <v>128</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_764380-MLU73463308040_122023-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_947113-MLB45202965881_032021-E.webp</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-futevolei-altinha-ftv-ft5-penta-futemesa-rio-cor-preto/p/MLB29123039#polycard_client=search-nordic&amp;searchVariation=MLB29123039&amp;wid=MLB4321183772&amp;position=28&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-81-dalponte-star-campo-costurada-a-mo-original/p/MLB20563342?searchVariation=MLB20563342#polycard_client=search-nordic&amp;searchVariation=MLB20563342&amp;wid=MLB4006264629&amp;position=37&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Bola 81 Dalponte Star Campo Costurada A Mão Original</t>
+          <t>Bola Futevolei Altinha Ftv Ft5 Penta Futemesa Rio Footvoley Super PU Cor Amarelo</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_947113-MLB45202965881_032021-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_905834-MLA83851667349_042025-E.webp</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-81-dalponte-star-campo-costurada-a-mo-original/p/MLB20563342#polycard_client=search-nordic&amp;searchVariation=MLB20563342&amp;wid=MLB4006264629&amp;position=26&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-futevolei-altinha-ftv-ft5-penta-futemesa-rio-footvoley-super-pu-cor-amarelo/p/MLB29146288?searchVariation=MLB29146288#polycard_client=search-nordic&amp;searchVariation=MLB29146288&amp;wid=MLB4321183780&amp;position=30&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bola de futevolei Poker Rio Poker nº 5 Unidade x 1 unidades cor rosa e preto</t>
+          <t>Bola De Futebol Society Kappa Player + Bomba De Ar</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>135</v>
+        <v>132.9</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_904045-MLU79036618824_092024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_877613-MLB84075225265_042025-E-bola-de-futebol-society-kappa-player-bomba-de-ar.webp</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-unidade-x-1-unidades-cor-rosa-e-preto/p/MLB19698706#polycard_client=search-nordic&amp;searchVariation=MLB19698706&amp;wid=MLB5051108460&amp;position=34&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-5365605436-bola-de-futebol-society-kappa-player-bomba-de-ar-_JM?searchVariation=183447294694#polycard_client=search-nordic&amp;searchVariation=183447294694&amp;position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Bola de Futevolei Poker Rio Poker nº 5 cor amarelo e preto</t>
+          <t>Bola de futebol Dalponte nº 70 Unidade x 1 unidades cor branco</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>139.29</v>
+        <v>133.22</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_753390-MLU74696438844_022024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_730532-MLU75289033019_032024-E.webp</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-cor-amarelo-e-preto/p/MLB19698709#polycard_client=search-nordic&amp;searchVariation=MLB19698709&amp;wid=MLB3889075523&amp;position=31&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-dalponte-n-70-unidade-x-1-unidades-cor-branco/p/MLB22996803?searchVariation=MLB22996803#polycard_client=search-nordic&amp;searchVariation=MLB22996803&amp;wid=MLB3304776185&amp;position=33&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>140.11</v>
+        <v>137.93</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1258,207 +1258,207 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-unidade-x-1-unidades-cor-branco-e-preto/p/MLB19698708#polycard_client=search-nordic&amp;searchVariation=MLB19698708&amp;wid=MLB3889079001&amp;position=33&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-unidade-x-1-unidades-cor-branco-e-preto/p/MLB19698708?searchVariation=MLB19698708#polycard_client=search-nordic&amp;searchVariation=MLB19698708&amp;wid=MLB5338642928&amp;position=24&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bola Futevôlei Vulcanizada Pu Poker Original Branca/azul</t>
+          <t>Bola De Futevôlei Altinha Poker Rio N° 5 Esporte Praia Pro Cor Branca e Laranja</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>149.9</v>
+        <v>137.93</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_601980-MLB83086122841_032025-E-bola-futevlei-vulcanizada-pu-poker-original-brancaazul.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_740496-MLA84473749359_052025-E.webp</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-5318075606-bola-futevlei-vulcanizada-pu-poker-original-brancaazul-_JM#polycard_client=search-nordic&amp;position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevlei-altinha-poker-rio-n-5-esporte-praia-pro-cor-branca-e-laranja/p/MLB24350523?searchVariation=MLB24350523#polycard_client=search-nordic&amp;searchVariation=MLB24350523&amp;wid=MLB4006415601&amp;position=25&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bola De Futebol Society 8 X Penalty</t>
+          <t>Bola de futevolei Poker Rio Poker nº 5 Unidade x 1 unidades cor rosa e azul marinho</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>154.71</v>
+        <v>137.93</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_818310-MLU76366734942_052024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_904045-MLU79036618824_092024-E.webp</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-society-8-x-penalty/p/MLB19776132#polycard_client=search-nordic&amp;searchVariation=MLB19776132&amp;wid=MLB3829143887&amp;position=15&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevolei-poker-rio-poker-n-5-unidade-x-1-unidades-cor-rosa-e-azul-marinho/p/MLB19698706?searchVariation=MLB19698706#polycard_client=search-nordic&amp;searchVariation=MLB19698706&amp;wid=MLB4006299477&amp;position=31&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bola De Futebol Campo Uhlsport Match R1 Brasileirão 2025</t>
+          <t>Bola De Futevôlei Poker Rio Ftv-5 Pro</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>155.99</v>
+        <v>137.93</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_857447-MLB82813326112_032025-E-bola-de-futebol-campo-uhlsport-match-r1-brasileiro-2025.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_718503-MLU75290479961_032024-E.webp</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-4003764129-bola-de-futebol-campo-uhlsport-match-r1-brasileiro-2025-_JM#polycard_client=search-nordic&amp;position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futevlei-poker-rio-ftv-5-pro/p/MLB27949636?searchVariation=MLB27949636#polycard_client=search-nordic&amp;searchVariation=MLB27949636&amp;wid=MLB3596574425&amp;position=41&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bola De Campo Penalty S11 R2 Xxv ( Camp.paulista)</t>
+          <t>Bola Futebol De Salão Futsal Dalponte 81 Costurada</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>159.9</v>
+        <v>139.4</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_687100-MLB82940622023_032025-E-bola-de-campo-penalty-s11-r2-xxv-camppaulista.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_949578-MLU72859154453_112023-E.webp</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3996246671-bola-de-campo-penalty-s11-r2-xxv-camppaulista-_JM?searchVariation=187147572233#polycard_client=search-nordic&amp;searchVariation=187147572233&amp;position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-futebol-de-salo-futsal-dalponte-81-costurada/p/MLB24560282?searchVariation=MLB24560282#polycard_client=search-nordic&amp;searchVariation=MLB24560282&amp;wid=MLB3468247509&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bola Futebol De Campo Bola 8 Penalty Cor Preto</t>
+          <t>Kagiva Profissional F5 Branco 2022 64</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>164</v>
+        <v>150.5</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_888107-MLA81942694869_012025-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_912769-MLU74696060400_022024-E.webp</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-futebol-de-campo-bola-8-penalty-cor-preto/p/MLB22210458#polycard_client=search-nordic&amp;searchVariation=MLB22210458&amp;wid=MLB3945165169&amp;position=37&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/kagiva-profissional-f5-branco-2022-64/p/MLB19754377?searchVariation=MLB19754377#polycard_client=search-nordic&amp;searchVariation=MLB19754377&amp;wid=MLB4540427612&amp;position=44&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Bola De Futebol Dalponte 81 Nitro Society Costurada À Mão Cor Branco</t>
+          <t>Bola De Futebol Society 8 X Penalty</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>176.62</v>
+        <v>157.53</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_756582-MLU74393181908_022024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_818310-MLU76366734942_052024-E.webp</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futebol-dalponte-81-nitro-society-costurada-mo-cor-branco/p/MLB32946547#polycard_client=search-nordic&amp;searchVariation=MLB32946547&amp;wid=MLB3596272369&amp;position=21&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futebol-society-8-x-penalty/p/MLB19776132?searchVariation=MLB19776132#polycard_client=search-nordic&amp;searchVariation=MLB19776132&amp;wid=MLB4128367346&amp;position=12&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Bola Futebol Society 8 Pro Xxiv Tamanho 5 Cor Preto e Branco Penalty</t>
+          <t>Bola Futebol Society Dalponte Alpha Verde E Marinho Society</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>297</v>
+        <v>172</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_819669-MLU75482475121_032024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_955981-MLB84217672272_052025-E-bola-futebol-society-dalponte-alpha-verde-e-marinho-society.webp</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-futebol-society-8-pro-xxiv-tamanho-5-cor-preto-e-branco-penalty/p/MLB35142675#polycard_client=search-nordic&amp;searchVariation=MLB35142675&amp;wid=MLB4630087278&amp;position=14&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://produto.mercadolivre.com.br/MLB-4057576185-bola-futebol-society-dalponte-alpha-verde-e-marinho-society-_JM?searchVariation=187880594707#polycard_client=search-nordic&amp;searchVariation=187880594707&amp;position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Bola De Futsal Penalty Max 1000 Xxiv Cor Azul</t>
+          <t>Bola Society 8 X Amarelo, Branco E Preto Penalty</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>298.28</v>
+        <v>185</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_973308-MLU75866936168_042024-E.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_692679-MLA80330996332_112024-E.webp</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/bola-de-futsal-penalty-max-1000-xxiv-cor-azul/p/MLB36227619#polycard_client=search-nordic&amp;searchVariation=MLB36227619&amp;wid=MLB3937932227&amp;position=25&amp;search_layout=grid&amp;type=product&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d&amp;sid=search</t>
+          <t>https://www.mercadolivre.com.br/bola-society-8-x-amarelo-branco-e-preto-penalty/p/MLB19719046?searchVariation=MLB19719046#polycard_client=search-nordic&amp;searchVariation=MLB19719046&amp;wid=MLB3955181335&amp;position=20&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Bola Uhlsport Campo Game Pro Brasileirão Série C E D 2025</t>
+          <t>Conjunto De Jogos Para Diversão Na Praia, No Jardim E Ao Ar</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>379</v>
+        <v>215.4</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_652481-MLB82865558482_032025-E-bola-uhlsport-campo-game-pro-brasileiro-serie-c-e-d-2025.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_653456-CBT84582210979_052025-E.webp</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-4006258699-bola-uhlsport-campo-game-pro-brasileiro-serie-c-e-d-2025-_JM?searchVariation=187252357205#polycard_client=search-nordic&amp;searchVariation=187252357205&amp;position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/game-set-for-beach-yardoutdoor-fun-complete-kit-for-kids/p/MLB2017925542#polycard_client=search-nordic&amp;searchVariation=MLB2017925542&amp;wid=MLB5384145428&amp;position=4&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Kit 50 Bolas Futebol Couro Sintético Costurada N°05</t>
+          <t>Bola De Futsal Penalty Max 1000 Xxiv Cor Azul</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>916</v>
+        <v>254.24</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://http2.mlstatic.com/D_Q_NP_2X_871334-MLB82990085837_032025-E-kit-50-bolas-futebol-couro-sintetico-costurada-n05.webp</t>
+          <t>https://http2.mlstatic.com/D_Q_NP_2X_809733-MLA83760374857_042025-E.webp</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-5313103164-kit-50-bolas-futebol-couro-sintetico-costurada-n05-_JM?searchVariation=183096595076#polycard_client=search-nordic&amp;searchVariation=183096595076&amp;position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=8e611849-75a7-4304-8cbe-30b2b6ffa88d</t>
+          <t>https://www.mercadolivre.com.br/bola-de-futsal-penalty-max-1000-xxiv-cor-azul/p/MLB36227619?searchVariation=MLB36227619#polycard_client=search-nordic&amp;searchVariation=MLB36227619&amp;wid=MLB3892608145&amp;position=7&amp;search_layout=grid&amp;type=product&amp;tracking_id=735c4488-9560-4c3f-be27-573d812e2714&amp;sid=search</t>
         </is>
       </c>
     </row>

</xml_diff>